<commit_message>
testing rmarkdown and metadata file
</commit_message>
<xml_diff>
--- a/test_scripts/metadata.xlsx
+++ b/test_scripts/metadata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -435,7 +435,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -446,146 +446,145 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3">
-        <v>0.91666666666666696</v>
+        <v>2.4833333333332988</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>1.93333333333333</v>
+        <v>3.3999999999999657</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>1.93333333333333</v>
+        <v>4.4166666666666288</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>2.93333333333333</v>
+        <v>4.4166666666666288</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>2.93333333333333</v>
+        <v>5.4166666666666288</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8">
-        <v>3.9166666666666701</v>
+        <v>5.4166666666666288</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>4.9000000000000004</v>
+        <v>6.3999999999999684</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>4.9000000000000004</v>
+        <v>7.3833333333332991</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11">
-        <v>6.1666666666666696</v>
+        <v>7.3833333333332991</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12">
-        <v>6.9666666666666703</v>
+        <v>8.6499999999999684</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
       <c r="C13">
-        <v>7.93333333333333</v>
+        <v>9.4499999999999691</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
       <c r="C14">
-        <v>8.9833333333333307</v>
+        <v>10.416666666666629</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
       <c r="C15">
-        <f>21.5166666666667-24</f>
-        <v>-2.4833333333332988</v>
+        <v>11.466666666666629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>